<commit_message>
successfully saved the model to a file using pickle then imported it and predicted, got the same accruacy as before
</commit_message>
<xml_diff>
--- a/regression-training-data/PriceData.xlsx
+++ b/regression-training-data/PriceData.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21818"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB082FBC-BAA7-4B99-A9F3-E778025FB29D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70CED484-3175-4409-AE90-DF3F7299F876}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SimpleData" sheetId="1" r:id="rId1"/>
-    <sheet name="DetailedData" sheetId="3" r:id="rId2"/>
-    <sheet name="Factors" sheetId="2" r:id="rId3"/>
+    <sheet name="SeasonalData" sheetId="4" r:id="rId1"/>
+    <sheet name="SimpleData" sheetId="1" r:id="rId2"/>
+    <sheet name="DetailedData" sheetId="3" r:id="rId3"/>
+    <sheet name="Factors" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -84,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Price per Square meter</t>
   </si>
@@ -92,6 +93,18 @@
     <t>StartDate</t>
   </si>
   <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
     <t>MinimumWage</t>
   </si>
   <si>
@@ -170,6 +183,9 @@
     <t>Type</t>
   </si>
   <si>
+    <t>"Synthetic but realistic"</t>
+  </si>
+  <si>
     <t>Season</t>
   </si>
   <si>
@@ -195,6 +211,9 @@
   </si>
   <si>
     <t>20 clay</t>
+  </si>
+  <si>
+    <t>https://www.thespruce.com/best-roofing-materials-for-longevity-1821951</t>
   </si>
   <si>
     <t>Structural damage</t>
@@ -228,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,9 +256,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -271,15 +306,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -291,8 +327,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -635,11 +674,2287 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4696AE80-C151-4207-B9C6-B70E36BADBE9}">
+  <dimension ref="A1:N51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="5">
+        <v>50</v>
+      </c>
+      <c r="B2" s="6">
+        <v>43466</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H2" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="5">
+        <v>190</v>
+      </c>
+      <c r="B3" s="6">
+        <v>43466</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="5">
+        <v>295</v>
+      </c>
+      <c r="B4" s="6">
+        <v>43466</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="5">
+        <v>450</v>
+      </c>
+      <c r="B5" s="6">
+        <v>43466</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H5" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="5">
+        <v>59</v>
+      </c>
+      <c r="B6" s="6">
+        <v>43497</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H6" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="5">
+        <v>241</v>
+      </c>
+      <c r="B7" s="6">
+        <v>43497</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="5">
+        <v>365</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43497</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H8" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="5">
+        <v>490</v>
+      </c>
+      <c r="B9" s="6">
+        <v>43497</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="5">
+        <v>78</v>
+      </c>
+      <c r="B10" s="6">
+        <v>43525</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="5">
+        <v>300</v>
+      </c>
+      <c r="B11" s="6">
+        <v>43525</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H11" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="5">
+        <v>542</v>
+      </c>
+      <c r="B12" s="6">
+        <v>43525</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H12" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="5">
+        <v>705</v>
+      </c>
+      <c r="B13" s="6">
+        <v>43525</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="5">
+        <v>62</v>
+      </c>
+      <c r="B14" s="6">
+        <v>43435</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H14" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="5">
+        <v>240</v>
+      </c>
+      <c r="B15" s="6">
+        <v>43435</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="5">
+        <v>360</v>
+      </c>
+      <c r="B16" s="6">
+        <v>43435</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H16" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="5">
+        <v>400</v>
+      </c>
+      <c r="B17" s="6">
+        <v>43435</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H17" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="5">
+        <v>48</v>
+      </c>
+      <c r="B18" s="6">
+        <v>43405</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H18" s="5">
+        <v>4</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="5">
+        <v>45</v>
+      </c>
+      <c r="B19" s="6">
+        <v>43374</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H19" s="5">
+        <v>4</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="5">
+        <v>67</v>
+      </c>
+      <c r="B20" s="6">
+        <v>43374</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H20" s="5">
+        <v>4</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="5">
+        <v>51</v>
+      </c>
+      <c r="B21" s="6">
+        <v>43374</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H21" s="5">
+        <v>4</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="5">
+        <v>42</v>
+      </c>
+      <c r="B22" s="6">
+        <v>43344</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H22" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="5">
+        <v>40</v>
+      </c>
+      <c r="B23" s="6">
+        <v>43313</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="5">
+        <v>160</v>
+      </c>
+      <c r="B24" s="6">
+        <v>43313</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H24" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="5">
+        <v>250</v>
+      </c>
+      <c r="B25" s="6">
+        <v>43313</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H25" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="5">
+        <v>360</v>
+      </c>
+      <c r="B26" s="6">
+        <v>43313</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H26" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="5">
+        <v>61</v>
+      </c>
+      <c r="B27" s="6">
+        <v>43282</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H27" s="5">
+        <v>4</v>
+      </c>
+      <c r="I27" s="5">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="5">
+        <v>245</v>
+      </c>
+      <c r="B28" s="6">
+        <v>43282</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H28" s="5">
+        <v>4</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="5">
+        <v>336</v>
+      </c>
+      <c r="B29" s="6">
+        <v>43282</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H29" s="5">
+        <v>4</v>
+      </c>
+      <c r="I29" s="5">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
+        <v>1</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="5">
+        <v>530</v>
+      </c>
+      <c r="B30" s="6">
+        <v>43282</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H30" s="5">
+        <v>4</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5">
+        <v>1</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="5">
+        <v>45</v>
+      </c>
+      <c r="B31" s="6">
+        <v>43252</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H31" s="5">
+        <v>4</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="5">
+        <v>170</v>
+      </c>
+      <c r="B32" s="6">
+        <v>43252</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H32" s="5">
+        <v>4</v>
+      </c>
+      <c r="I32" s="5">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="5">
+        <v>290</v>
+      </c>
+      <c r="B33" s="6">
+        <v>43252</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H33" s="5">
+        <v>4</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <v>0</v>
+      </c>
+      <c r="M33" s="4">
+        <v>1</v>
+      </c>
+      <c r="N33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="5">
+        <v>450</v>
+      </c>
+      <c r="B34" s="6">
+        <v>43252</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H34" s="5">
+        <v>4</v>
+      </c>
+      <c r="I34" s="5">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+      <c r="L34" s="4">
+        <v>0</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="5">
+        <v>43</v>
+      </c>
+      <c r="B35" s="6">
+        <v>43221</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H35" s="5">
+        <v>4</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4">
+        <v>0</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0</v>
+      </c>
+      <c r="N35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="5">
+        <v>66</v>
+      </c>
+      <c r="B36" s="6">
+        <v>43191</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H36" s="5">
+        <v>4</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1</v>
+      </c>
+      <c r="J36" s="5">
+        <v>1</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1</v>
+      </c>
+      <c r="L36" s="4">
+        <v>0</v>
+      </c>
+      <c r="M36" s="4">
+        <v>0</v>
+      </c>
+      <c r="N36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="5">
+        <v>265</v>
+      </c>
+      <c r="B37" s="6">
+        <v>43191</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H37" s="5">
+        <v>4</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1</v>
+      </c>
+      <c r="J37" s="5">
+        <v>1</v>
+      </c>
+      <c r="K37" s="4">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1</v>
+      </c>
+      <c r="M37" s="4">
+        <v>0</v>
+      </c>
+      <c r="N37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="5">
+        <v>445</v>
+      </c>
+      <c r="B38" s="6">
+        <v>43191</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H38" s="5">
+        <v>4</v>
+      </c>
+      <c r="I38" s="5">
+        <v>1</v>
+      </c>
+      <c r="J38" s="5">
+        <v>1</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0</v>
+      </c>
+      <c r="L38" s="4">
+        <v>0</v>
+      </c>
+      <c r="M38" s="4">
+        <v>1</v>
+      </c>
+      <c r="N38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="5">
+        <v>630</v>
+      </c>
+      <c r="B39" s="6">
+        <v>43191</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="H39" s="5">
+        <v>4</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5">
+        <v>1</v>
+      </c>
+      <c r="K39" s="4">
+        <v>0</v>
+      </c>
+      <c r="L39" s="4">
+        <v>0</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="5">
+        <v>56</v>
+      </c>
+      <c r="B40" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H40" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I40" s="5">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4">
+        <v>1</v>
+      </c>
+      <c r="L40" s="4">
+        <v>0</v>
+      </c>
+      <c r="M40" s="4">
+        <v>0</v>
+      </c>
+      <c r="N40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="5">
+        <v>200</v>
+      </c>
+      <c r="B41" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H41" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4">
+        <v>0</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4">
+        <v>0</v>
+      </c>
+      <c r="N41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="5">
+        <v>350</v>
+      </c>
+      <c r="B42" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H42" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4">
+        <v>0</v>
+      </c>
+      <c r="L42" s="4">
+        <v>0</v>
+      </c>
+      <c r="M42" s="4">
+        <v>1</v>
+      </c>
+      <c r="N42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="5">
+        <v>390</v>
+      </c>
+      <c r="B43" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H43" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <v>0</v>
+      </c>
+      <c r="L43" s="4">
+        <v>0</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0</v>
+      </c>
+      <c r="N43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="5">
+        <v>51</v>
+      </c>
+      <c r="B44" s="6">
+        <v>43132</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H44" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>1</v>
+      </c>
+      <c r="K44" s="4">
+        <v>1</v>
+      </c>
+      <c r="L44" s="4">
+        <v>0</v>
+      </c>
+      <c r="M44" s="4">
+        <v>0</v>
+      </c>
+      <c r="N44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="5">
+        <v>210</v>
+      </c>
+      <c r="B45" s="6">
+        <v>43132</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H45" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I45" s="5">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5">
+        <v>1</v>
+      </c>
+      <c r="K45" s="4">
+        <v>0</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0</v>
+      </c>
+      <c r="N45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="5">
+        <v>295</v>
+      </c>
+      <c r="B46" s="6">
+        <v>43132</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H46" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5">
+        <v>1</v>
+      </c>
+      <c r="K46" s="4">
+        <v>0</v>
+      </c>
+      <c r="L46" s="4">
+        <v>0</v>
+      </c>
+      <c r="M46" s="4">
+        <v>1</v>
+      </c>
+      <c r="N46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="5">
+        <v>485</v>
+      </c>
+      <c r="B47" s="6">
+        <v>43132</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H47" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I47" s="5">
+        <v>0</v>
+      </c>
+      <c r="J47" s="5">
+        <v>1</v>
+      </c>
+      <c r="K47" s="4">
+        <v>0</v>
+      </c>
+      <c r="L47" s="4">
+        <v>0</v>
+      </c>
+      <c r="M47" s="4">
+        <v>0</v>
+      </c>
+      <c r="N47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="5">
+        <v>75</v>
+      </c>
+      <c r="B48" s="6">
+        <v>43101</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H48" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1</v>
+      </c>
+      <c r="J48" s="5">
+        <v>1</v>
+      </c>
+      <c r="K48" s="4">
+        <v>1</v>
+      </c>
+      <c r="L48" s="4">
+        <v>0</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0</v>
+      </c>
+      <c r="N48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="5">
+        <v>278</v>
+      </c>
+      <c r="B49" s="6">
+        <v>43101</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H49" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1</v>
+      </c>
+      <c r="J49" s="5">
+        <v>1</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0</v>
+      </c>
+      <c r="L49" s="4">
+        <v>1</v>
+      </c>
+      <c r="M49" s="4">
+        <v>0</v>
+      </c>
+      <c r="N49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="5">
+        <v>450</v>
+      </c>
+      <c r="B50" s="6">
+        <v>43101</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H50" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1</v>
+      </c>
+      <c r="J50" s="5">
+        <v>1</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0</v>
+      </c>
+      <c r="L50" s="4">
+        <v>0</v>
+      </c>
+      <c r="M50" s="4">
+        <v>1</v>
+      </c>
+      <c r="N50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="5">
+        <v>650</v>
+      </c>
+      <c r="B51" s="6">
+        <v>43101</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="H51" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1</v>
+      </c>
+      <c r="J51" s="5">
+        <v>1</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0</v>
+      </c>
+      <c r="L51" s="4">
+        <v>0</v>
+      </c>
+      <c r="M51" s="4">
+        <v>0</v>
+      </c>
+      <c r="N51" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -660,28 +2975,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2289,7 +4604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D32D2D-DF80-469E-980C-92936B6365C5}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -2309,52 +4624,52 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="P1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="Q1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2442,12 +4757,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB75EA5-C465-44C7-AF73-C7A9A2CB0DF9}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2455,67 +4770,73 @@
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
       <c r="D6">
         <v>2.25</v>
@@ -2530,67 +4851,70 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{870A5C7F-6AD5-4122-A6AE-7CA3F8F03442}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>